<commit_message>
Small fix to 1, don't think it's fully working yet though
</commit_message>
<xml_diff>
--- a/fogos1/fogos1.xlsx
+++ b/fogos1/fogos1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A91941A-7DEA-48C3-9F5A-2FF3C4961A08}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D61F1-E8BB-486B-A8DF-8B3A7E116D30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6900" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="b">Sheet1!$B$4</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Norte</t>
   </si>
@@ -469,7 +470,7 @@
   <dimension ref="A2:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28:Q34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,60 +497,46 @@
         <v>8</v>
       </c>
       <c r="C3" s="1">
-        <f ca="1">8+RANDBETWEEN(1,3)</f>
         <v>9</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:I9" ca="1" si="0">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K3" s="2">
-        <f ca="1">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:Q9" ca="1" si="1">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="Q3" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -560,350 +547,266 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C9" ca="1" si="2">8+RANDBETWEEN(1,3)</f>
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K9" ca="1" si="3">8+RANDBETWEEN(1,3)</f>
         <v>10</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
-        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="N5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
-        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" ca="1" si="3"/>
         <v>11</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O6" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="P6" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
-        <f t="shared" ca="1" si="2"/>
         <v>10</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="P7" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="O8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P8" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>10</v>
       </c>
       <c r="Q8" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
-        <f t="shared" ca="1" si="2"/>
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" ca="1" si="1"/>
         <v>9</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -916,407 +819,309 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" s="3">
-        <f ca="1">1+RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" ref="D12:I18" ca="1" si="4">1+RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I12" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" s="4">
-        <f ca="1">6+RANDBETWEEN(1,3)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12:Q18" ca="1" si="5">6+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" s="3">
-        <f t="shared" ref="C13:C18" ca="1" si="6">1+RANDBETWEEN(1,3)</f>
         <v>4</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I13" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" ref="K13:K18" ca="1" si="7">6+RANDBETWEEN(1,3)</f>
         <v>9</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M13" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N13" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
       <c r="O13" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
-        <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F14" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="G14" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" ca="1" si="7"/>
         <v>9</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>7</v>
       </c>
       <c r="O14" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q14" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" ca="1" si="7"/>
         <v>7</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" s="3">
-        <f t="shared" ca="1" si="6"/>
         <v>3</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="I16" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O16" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>7</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>8</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C17" s="3">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>3</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" ca="1" si="7"/>
         <v>7</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O17" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C18" s="3">
-        <f t="shared" ca="1" si="6"/>
         <v>4</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>4</v>
       </c>
       <c r="F18" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" ca="1" si="4"/>
         <v>2</v>
       </c>
       <c r="I18" s="3">
-        <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>7</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" ca="1" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -1349,22 +1154,22 @@
         <v>9</v>
       </c>
       <c r="K20" s="5">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="L20" s="5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="M20" s="5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N20" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O20" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P20" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="5">
         <v>0</v>
@@ -1393,19 +1198,19 @@
         <v>0</v>
       </c>
       <c r="K21" s="5">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="5">
         <v>1</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0</v>
-      </c>
-      <c r="M21" s="5">
-        <v>0</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0</v>
       </c>
       <c r="P21" s="5">
         <v>0</v>
@@ -1437,22 +1242,22 @@
         <v>0</v>
       </c>
       <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5">
+        <v>18</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="5">
+        <v>2</v>
+      </c>
+      <c r="P22" s="5">
         <v>1</v>
-      </c>
-      <c r="L22" s="5">
-        <v>0</v>
-      </c>
-      <c r="M22" s="5">
-        <v>0</v>
-      </c>
-      <c r="N22" s="5">
-        <v>0</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
-      <c r="P22" s="5">
-        <v>0</v>
       </c>
       <c r="Q22" s="5">
         <v>0</v>
@@ -1487,16 +1292,16 @@
         <v>0</v>
       </c>
       <c r="M23" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N23" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O23" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="5">
         <v>0</v>
@@ -1531,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="5">
         <v>0</v>
@@ -1540,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q24" s="5">
         <v>0</v>
@@ -1569,16 +1374,16 @@
         <v>0</v>
       </c>
       <c r="K25" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L25" s="5">
         <v>0</v>
       </c>
       <c r="M25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="5">
         <v>0</v>
@@ -1595,40 +1400,40 @@
         <v>0</v>
       </c>
       <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0</v>
+      </c>
+      <c r="I26" s="5">
+        <v>0</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0</v>
+      </c>
+      <c r="L26" s="5">
+        <v>3</v>
+      </c>
+      <c r="M26" s="5">
+        <v>2</v>
+      </c>
+      <c r="N26" s="5">
         <v>1</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
-        <v>0</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
-      <c r="I26" s="5">
-        <v>0</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0</v>
-      </c>
-      <c r="L26" s="5">
-        <v>0</v>
-      </c>
-      <c r="M26" s="5">
-        <v>0</v>
-      </c>
-      <c r="N26" s="5">
-        <v>0</v>
-      </c>
       <c r="O26" s="5">
         <v>0</v>
       </c>
       <c r="P26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q26" s="5">
         <v>0</v>
@@ -1639,46 +1444,46 @@
         <v>8</v>
       </c>
       <c r="C28" s="5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H28" s="5">
         <v>0</v>
       </c>
       <c r="I28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="5">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="L28" s="5">
         <v>0</v>
       </c>
       <c r="M28" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N28" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O28" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P28" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="5">
         <v>0</v>
@@ -1686,22 +1491,22 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C29" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D29" s="5">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="5">
         <v>0</v>
@@ -1713,16 +1518,16 @@
         <v>0</v>
       </c>
       <c r="M29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="5">
         <v>0</v>
@@ -1730,13 +1535,13 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D30" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30" s="5">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F30" s="5">
         <v>0</v>
@@ -1745,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="5">
         <v>0</v>
@@ -1766,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="5">
         <v>0</v>
@@ -1774,22 +1579,22 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F31" s="5">
         <v>0</v>
       </c>
       <c r="G31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I31" s="5">
         <v>0</v>
@@ -1818,25 +1623,25 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F32" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -1862,25 +1667,25 @@
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E33" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G33" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -1909,19 +1714,19 @@
         <v>0</v>
       </c>
       <c r="D34" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E34" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F34" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G34" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H34" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I34" s="5">
         <v>0</v>
@@ -1933,13 +1738,13 @@
         <v>0</v>
       </c>
       <c r="M34" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O34" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" s="5">
         <v>0</v>
@@ -1952,4 +1757,839 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6038AB6C-12B6-4FDE-BC21-38432BDEFD6C}">
+  <dimension ref="B2:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <f ca="1">8+RANDBETWEEN(1,3)</f>
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <f t="shared" ref="C2:H8" ca="1" si="0">8+RANDBETWEEN(1,3)</f>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <f ca="1">8+RANDBETWEEN(1,3)</f>
+        <v>9</v>
+      </c>
+      <c r="K2" s="2">
+        <f t="shared" ref="K2:P8" ca="1" si="1">8+RANDBETWEEN(1,3)</f>
+        <v>10</v>
+      </c>
+      <c r="L2" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M2" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O2" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P2" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B8" ca="1" si="2">8+RANDBETWEEN(1,3)</f>
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J3" s="2">
+        <f t="shared" ref="J3:J8" ca="1" si="3">8+RANDBETWEEN(1,3)</f>
+        <v>11</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="O3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P3" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="J6" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <f ca="1">1+RANDBETWEEN(1,3)</f>
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" ref="C11:H17" ca="1" si="4">1+RANDBETWEEN(1,3)</f>
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="J11" s="4">
+        <f ca="1">6+RANDBETWEEN(1,3)</f>
+        <v>9</v>
+      </c>
+      <c r="K11" s="4">
+        <f t="shared" ref="K11:P17" ca="1" si="5">6+RANDBETWEEN(1,3)</f>
+        <v>8</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <f t="shared" ref="B12:B17" ca="1" si="6">1+RANDBETWEEN(1,3)</f>
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ref="J12:J17" ca="1" si="7">6+RANDBETWEEN(1,3)</f>
+        <v>7</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="M15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="M16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <f t="shared" ca="1" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="M17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="N17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Problema 1a IS WORKING BITCHEZ
</commit_message>
<xml_diff>
--- a/fogos1/fogos1.xlsx
+++ b/fogos1/fogos1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D61F1-E8BB-486B-A8DF-8B3A7E116D30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E59BD-A084-45B4-87E6-1D72FB032DD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6900" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
@@ -1154,22 +1154,22 @@
         <v>9</v>
       </c>
       <c r="K20" s="5">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="L20" s="5">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="M20" s="5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N20" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="O20" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P20" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="5">
         <v>0</v>
@@ -1198,25 +1198,25 @@
         <v>0</v>
       </c>
       <c r="K21" s="5">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L21" s="5">
         <v>0</v>
       </c>
       <c r="M21" s="5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N21" s="5">
         <v>0</v>
       </c>
       <c r="O21" s="5">
+        <v>0</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="5">
         <v>1</v>
-      </c>
-      <c r="P21" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="5">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
@@ -1242,22 +1242,22 @@
         <v>0</v>
       </c>
       <c r="K22" s="5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L22" s="5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M22" s="5">
         <v>0</v>
       </c>
       <c r="N22" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O22" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="P22" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q22" s="5">
         <v>0</v>
@@ -1286,25 +1286,25 @@
         <v>0</v>
       </c>
       <c r="K23" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L23" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M23" s="5">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N23" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="O23" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="P23" s="5">
         <v>1</v>
       </c>
       <c r="Q23" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
@@ -1330,22 +1330,22 @@
         <v>0</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="5">
         <v>1</v>
       </c>
-      <c r="N24" s="5">
-        <v>0</v>
-      </c>
       <c r="O24" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P24" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q24" s="5">
         <v>0</v>
@@ -1374,22 +1374,22 @@
         <v>0</v>
       </c>
       <c r="K25" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="5">
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q25" s="5">
         <v>0</v>
@@ -1421,13 +1421,13 @@
         <v>0</v>
       </c>
       <c r="L26" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M26" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="5">
         <v>0</v>
@@ -1444,25 +1444,25 @@
         <v>8</v>
       </c>
       <c r="C28" s="5">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D28" s="5">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E28" s="5">
+        <v>4</v>
+      </c>
+      <c r="F28" s="5">
+        <v>3</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="5">
-        <v>2</v>
-      </c>
-      <c r="G28" s="5">
-        <v>5</v>
-      </c>
-      <c r="H28" s="5">
-        <v>0</v>
-      </c>
       <c r="I28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="s">
         <v>10</v>
@@ -1491,22 +1491,22 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C29" s="5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D29" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E29" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F29" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G29" s="5">
         <v>3</v>
       </c>
       <c r="H29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" s="5">
         <v>0</v>
@@ -1535,19 +1535,19 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C30" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D30" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E30" s="5">
         <v>17</v>
       </c>
       <c r="F30" s="5">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G30" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H30" s="5">
         <v>0</v>
@@ -1579,22 +1579,22 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C31" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D31" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F31" s="5">
         <v>0</v>
       </c>
       <c r="G31" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I31" s="5">
         <v>0</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
       </c>
       <c r="E32" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32" s="5">
         <v>0</v>
@@ -1638,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="H32" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I32" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K32" s="5">
         <v>0</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="5">
         <v>4</v>
@@ -1679,13 +1679,13 @@
         <v>0</v>
       </c>
       <c r="G33" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H33" s="5">
         <v>1</v>
       </c>
       <c r="I33" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" s="5">
         <v>0</v>
@@ -1717,16 +1717,16 @@
         <v>0</v>
       </c>
       <c r="E34" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="5">
         <v>0</v>
       </c>
       <c r="H34" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="5">
         <v>0</v>
@@ -1772,7 +1772,7 @@
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <f ca="1">8+RANDBETWEEN(1,3)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:H8" ca="1" si="0">8+RANDBETWEEN(1,3)</f>
@@ -1780,11 +1780,11 @@
       </c>
       <c r="D2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1792,35 +1792,35 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2">
         <f ca="1">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:P8" ca="1" si="1">8+RANDBETWEEN(1,3)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1830,15 +1830,15 @@
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f t="shared" ref="B3:B8" ca="1" si="2">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1850,23 +1850,23 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J8" ca="1" si="3">8+RANDBETWEEN(1,3)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1874,15 +1874,15 @@
       </c>
       <c r="N3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
@@ -1892,39 +1892,39 @@
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1936,17 +1936,17 @@
       </c>
       <c r="O4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1962,35 +1962,35 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1998,21 +1998,21 @@
       </c>
       <c r="P5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2024,23 +2024,23 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2048,33 +2048,33 @@
       </c>
       <c r="N6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2082,23 +2082,23 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2106,11 +2106,11 @@
       </c>
       <c r="N7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P7" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2132,7 +2132,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2156,7 +2156,7 @@
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="N8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="P8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -2190,11 +2190,11 @@
       </c>
       <c r="C11" s="3">
         <f t="shared" ref="C11:H17" ca="1" si="4">1+RANDBETWEEN(1,3)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2210,15 +2210,15 @@
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J11" s="4">
         <f ca="1">6+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" ref="K11:P17" ca="1" si="5">6+RANDBETWEEN(1,3)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="O11" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2244,7 +2244,7 @@
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B17" ca="1" si="6">1+RANDBETWEEN(1,3)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2252,27 +2252,27 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" ref="J12:J17" ca="1" si="7">6+RANDBETWEEN(1,3)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2284,7 +2284,7 @@
       </c>
       <c r="M12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="O12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2302,7 +2302,7 @@
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2314,7 +2314,7 @@
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="G13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2330,15 +2330,15 @@
       </c>
       <c r="J13" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2346,11 +2346,11 @@
       </c>
       <c r="N13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2360,15 +2360,15 @@
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2376,11 +2376,11 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2388,45 +2388,45 @@
       </c>
       <c r="J14" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2434,15 +2434,15 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" ca="1" si="7"/>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="L15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2462,11 +2462,11 @@
       </c>
       <c r="N15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2480,23 +2480,23 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2504,69 +2504,69 @@
       </c>
       <c r="J16" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2578,15 +2578,15 @@
       </c>
       <c r="N17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização final com zip para enviar
</commit_message>
<xml_diff>
--- a/fogos1/fogos1.xlsx
+++ b/fogos1/fogos1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84E59BD-A084-45B4-87E6-1D72FB032DD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD94C476-E0E7-4A0D-B7AC-B4ECDA1254F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="6900" xr2:uid="{63F9166B-6F17-4C5E-B7E0-12EB27E8F6D8}"/>
   </bookViews>
@@ -1772,15 +1772,15 @@
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <f ca="1">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:H8" ca="1" si="0">8+RANDBETWEEN(1,3)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="F2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1804,11 +1804,11 @@
       </c>
       <c r="K2" s="2">
         <f t="shared" ref="K2:P8" ca="1" si="1">8+RANDBETWEEN(1,3)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1816,21 +1816,21 @@
       </c>
       <c r="N2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P2" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <f t="shared" ref="B3:B8" ca="1" si="2">8+RANDBETWEEN(1,3)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="H3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J8" ca="1" si="3">8+RANDBETWEEN(1,3)</f>
@@ -1862,11 +1862,11 @@
       </c>
       <c r="K3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="N3" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1888,11 +1888,11 @@
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1916,11 +1916,11 @@
       </c>
       <c r="J4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1928,29 +1928,29 @@
       </c>
       <c r="M4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1962,11 +1962,11 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -1974,11 +1974,11 @@
       </c>
       <c r="J5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="O5" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2004,11 +2004,11 @@
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2016,23 +2016,23 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2040,23 +2040,23 @@
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -2066,23 +2066,23 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2094,15 +2094,15 @@
       </c>
       <c r="K7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2120,23 +2120,23 @@
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2156,11 +2156,11 @@
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" ca="1" si="1"/>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="P8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
@@ -2186,11 +2186,11 @@
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f ca="1">1+RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ref="C11:H17" ca="1" si="4">1+RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="J11" s="4">
         <f ca="1">6+RANDBETWEEN(1,3)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" ref="K11:P17" ca="1" si="5">6+RANDBETWEEN(1,3)</f>
@@ -2230,15 +2230,15 @@
       </c>
       <c r="N11" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -2248,15 +2248,15 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2264,11 +2264,11 @@
       </c>
       <c r="G12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" ref="J12:J17" ca="1" si="7">6+RANDBETWEEN(1,3)</f>
@@ -2284,15 +2284,15 @@
       </c>
       <c r="M12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O12" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P12" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2302,27 +2302,27 @@
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2330,27 +2330,27 @@
       </c>
       <c r="J13" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="N13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O13" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2364,11 +2364,11 @@
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2376,7 +2376,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2392,15 +2392,15 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2408,11 +2408,11 @@
       </c>
       <c r="O14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
@@ -2422,11 +2422,11 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2434,27 +2434,27 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2462,7 +2462,7 @@
       </c>
       <c r="N15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2470,41 +2470,41 @@
       </c>
       <c r="P15" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="L16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M16" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="N16" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O16" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2534,7 +2534,7 @@
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2546,11 +2546,11 @@
       </c>
       <c r="E17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" ca="1" si="4"/>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="J17" s="4">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2570,7 +2570,7 @@
       </c>
       <c r="L17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M17" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="N17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O17" s="4">
         <f t="shared" ca="1" si="5"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="P17" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>